<commit_message>
Updated stroop analysis Tuesday,mar31st
</commit_message>
<xml_diff>
--- a/Waldo_Stroop_Data/Waldo_stroop.xlsx
+++ b/Waldo_Stroop_Data/Waldo_stroop.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pennychen/Dropbox/waldo_experiment_files/Waldo_Stroop_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F508601C-8F89-2241-89A4-52DB25A8B7FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870CE083-4405-5240-9C70-1FF5A87578CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{AEBE0D70-CE59-1649-B3C9-BC1F2C82DE3A}"/>
+    <workbookView xWindow="-37620" yWindow="-5940" windowWidth="28040" windowHeight="16640" xr2:uid="{AEBE0D70-CE59-1649-B3C9-BC1F2C82DE3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Subject_id</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>acc_2</t>
+  </si>
+  <si>
+    <t>BI_0</t>
+  </si>
+  <si>
+    <t>BI_1</t>
   </si>
 </sst>
 </file>
@@ -405,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570351F4-F72D-3549-91BE-BE1BA39081DA}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K9" sqref="K9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,74 +441,259 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.40289999999999998</v>
+        <v>0.48352533365535499</v>
       </c>
       <c r="C2">
-        <v>0.35549999999999998</v>
+        <v>0.42909300128563399</v>
       </c>
       <c r="D2">
-        <v>0.39140000000000003</v>
+        <v>0.44610010709454301</v>
       </c>
       <c r="E2">
-        <v>0.79</v>
+        <v>0.97</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="G2">
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>0.97</v>
+      </c>
+      <c r="H2">
+        <f>D2-B2</f>
+        <v>-3.7425226560811986E-2</v>
+      </c>
+      <c r="I2">
+        <f>D2-C2</f>
+        <v>1.7007105808909018E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>0.40939999999999999</v>
+        <v>0.417529865529359</v>
       </c>
       <c r="C3">
-        <v>0.3795</v>
+        <v>0.40563969982942599</v>
       </c>
       <c r="D3">
-        <v>0.3982</v>
+        <v>0.410637058847998</v>
       </c>
       <c r="E3">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H9" si="0">D3-B3</f>
+        <v>-6.8928066813609967E-3</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I9" si="1">D3-C3</f>
+        <v>4.9973590185720118E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.47383718367516697</v>
+      </c>
+      <c r="C4">
+        <v>0.44230335605386001</v>
+      </c>
+      <c r="D4">
+        <v>0.45061710275209998</v>
+      </c>
+      <c r="E4">
+        <v>0.94</v>
+      </c>
+      <c r="F4">
         <v>0.99</v>
-      </c>
-      <c r="G3">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0.44769999999999999</v>
-      </c>
-      <c r="C4">
-        <v>0.38579999999999998</v>
-      </c>
-      <c r="D4">
-        <v>0.41349999999999998</v>
-      </c>
-      <c r="E4">
-        <v>0.89</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
       </c>
       <c r="G4">
         <v>0.99</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>-2.3220080923066988E-2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>8.3137466982399766E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.500284963090742</v>
+      </c>
+      <c r="C5">
+        <v>0.46159578989733901</v>
+      </c>
+      <c r="D5">
+        <v>0.48845917918963899</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>-1.1825783901103004E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>2.6863389292299977E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.36105030482545097</v>
+      </c>
+      <c r="C6">
+        <v>0.32340163772705199</v>
+      </c>
+      <c r="D6">
+        <v>0.32794953066301202</v>
+      </c>
+      <c r="E6">
+        <v>0.93</v>
+      </c>
+      <c r="F6">
+        <v>0.98</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>-3.3100774162438951E-2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>4.5478929359600295E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.34865799944741699</v>
+      </c>
+      <c r="C7">
+        <v>0.333351976229248</v>
+      </c>
+      <c r="D7">
+        <v>0.34045231838708101</v>
+      </c>
+      <c r="E7">
+        <v>0.88</v>
+      </c>
+      <c r="F7">
+        <v>0.98</v>
+      </c>
+      <c r="G7">
+        <v>0.95</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>-8.2056810603359787E-3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>7.1003421578330062E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.53755127486465404</v>
+      </c>
+      <c r="C8">
+        <v>0.454882532948647</v>
+      </c>
+      <c r="D8">
+        <v>0.49484324661663198</v>
+      </c>
+      <c r="E8">
+        <v>0.98</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>-4.2708028248022056E-2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>3.9960713667984982E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.43106960812087097</v>
+      </c>
+      <c r="C9">
+        <v>0.40777142501032199</v>
+      </c>
+      <c r="D9">
+        <v>0.40681328040001002</v>
+      </c>
+      <c r="E9">
+        <v>0.93</v>
+      </c>
+      <c r="F9">
+        <v>0.99</v>
+      </c>
+      <c r="G9">
+        <v>0.97</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-2.4256327720860948E-2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>-9.5814461031196174E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stroop data excel - final
</commit_message>
<xml_diff>
--- a/Waldo_Stroop_Data/Waldo_stroop.xlsx
+++ b/Waldo_Stroop_Data/Waldo_stroop.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pennychen/Dropbox/waldo_experiment_files/Waldo_Stroop_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449A53D5-EE51-C340-8ACB-1720862BDB42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3E63E6-304C-254C-AFCF-1A09E9FE345C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-7820" windowWidth="51200" windowHeight="28800" xr2:uid="{AEBE0D70-CE59-1649-B3C9-BC1F2C82DE3A}"/>
+    <workbookView xWindow="-44640" yWindow="-2800" windowWidth="28800" windowHeight="17540" xr2:uid="{AEBE0D70-CE59-1649-B3C9-BC1F2C82DE3A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Analysis" sheetId="2" r:id="rId1"/>
+    <sheet name="Raw" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
   <si>
     <t>con_0</t>
   </si>
@@ -120,6 +121,9 @@
   </si>
   <si>
     <t>BI_1_INV</t>
+  </si>
+  <si>
+    <t>MTD</t>
   </si>
 </sst>
 </file>
@@ -135,12 +139,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,8 +165,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,11 +481,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570351F4-F72D-3549-91BE-BE1BA39081DA}">
-  <dimension ref="A1:T11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB82728F-A95F-314A-9F0F-C94C7A4ADC35}">
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -543,42 +554,643 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>0.47889802916834801</v>
+        <v>0.55401448521567498</v>
       </c>
       <c r="D2">
-        <v>0.68185850819905403</v>
+        <v>0.50203217309239601</v>
       </c>
       <c r="E2">
-        <v>0.464976153345873</v>
+        <v>0.51133700948991401</v>
       </c>
       <c r="F2">
         <v>0.98</v>
       </c>
       <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>-4.2677475725760972E-2</v>
+      </c>
+      <c r="J2">
+        <v>9.3048363975180015E-3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>0.56624871091601903</v>
+      </c>
+      <c r="N2">
+        <v>0.56076166660782301</v>
+      </c>
+      <c r="O2">
+        <v>0.55884107654576798</v>
+      </c>
+      <c r="P2">
         <v>0.99</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
+      <c r="Q2">
+        <v>0.99</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>-7.4076343702510483E-3</v>
+      </c>
+      <c r="T2">
+        <v>-1.9205900620550276E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>0.417529865529359</v>
+      </c>
+      <c r="D3">
+        <v>0.40563969982942599</v>
+      </c>
+      <c r="E3">
+        <v>0.410637058847998</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>-6.8928066813609967E-3</v>
+      </c>
+      <c r="J3">
+        <v>4.9973590185720118E-3</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>0.38035551942913998</v>
+      </c>
+      <c r="N3">
+        <v>0.375436632708185</v>
+      </c>
+      <c r="O3">
+        <v>0.37663804515963401</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>-3.7174742695059715E-3</v>
+      </c>
+      <c r="T3">
+        <v>1.2014124514490021E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>0.500284963090742</v>
+      </c>
+      <c r="D4">
+        <v>0.46159578989733901</v>
+      </c>
+      <c r="E4">
+        <v>0.48845917918963899</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>-1.1825783901103004E-2</v>
+      </c>
+      <c r="J4">
+        <v>2.6863389292299977E-2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>0.46347544467607799</v>
+      </c>
+      <c r="N4">
+        <v>0.42595182342608801</v>
+      </c>
+      <c r="O4">
+        <v>0.45148728164304902</v>
+      </c>
+      <c r="P4">
+        <v>0.99</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>-1.1988163033028965E-2</v>
+      </c>
+      <c r="T4">
+        <v>2.5535458216961016E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>0.47450212521973301</v>
+      </c>
+      <c r="D5">
+        <v>0.44979111808264899</v>
+      </c>
+      <c r="E5">
+        <v>0.46438476795981598</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>-1.0117357259917026E-2</v>
+      </c>
+      <c r="J5">
+        <v>1.4593649877166992E-2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>0.47925778126947799</v>
+      </c>
+      <c r="N5">
+        <v>0.44576891401975099</v>
+      </c>
+      <c r="O5">
+        <v>0.45780706597903098</v>
+      </c>
+      <c r="P5">
+        <v>0.99</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>-2.1450715290447009E-2</v>
+      </c>
+      <c r="T5">
+        <v>1.2038151959279986E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>0.34865799944741699</v>
+      </c>
+      <c r="D6">
+        <v>0.333351976229248</v>
+      </c>
+      <c r="E6">
+        <v>0.34045231838708101</v>
+      </c>
+      <c r="F6">
+        <v>0.88</v>
+      </c>
+      <c r="G6">
+        <v>0.98</v>
+      </c>
+      <c r="H6">
+        <v>0.95</v>
+      </c>
+      <c r="I6">
+        <v>-8.2056810603359787E-3</v>
+      </c>
+      <c r="J6">
+        <v>7.1003421578330062E-3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>0.37286859355993901</v>
+      </c>
+      <c r="N6">
+        <v>0.36248020085932198</v>
+      </c>
+      <c r="O6">
+        <v>0.35991229872896202</v>
+      </c>
+      <c r="P6">
+        <v>0.91</v>
+      </c>
+      <c r="Q6">
+        <v>0.96</v>
+      </c>
+      <c r="R6">
+        <v>0.98</v>
+      </c>
+      <c r="S6">
+        <v>-1.2956294830976989E-2</v>
+      </c>
+      <c r="T6">
+        <v>-2.5679021303599558E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>0.53755127486465404</v>
+      </c>
+      <c r="D7">
+        <v>0.454882532948647</v>
+      </c>
+      <c r="E7">
+        <v>0.49484324661663198</v>
+      </c>
+      <c r="F7">
+        <v>0.98</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>-4.2708028248022056E-2</v>
+      </c>
+      <c r="J7">
+        <v>3.9960713667984982E-2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
+      </c>
+      <c r="M7">
+        <v>0.37286859355993901</v>
+      </c>
+      <c r="N7">
+        <v>0.36248020085932198</v>
+      </c>
+      <c r="O7">
+        <v>0.35991229872896202</v>
+      </c>
+      <c r="P7">
+        <v>0.91</v>
+      </c>
+      <c r="Q7">
+        <v>0.96</v>
+      </c>
+      <c r="R7">
+        <v>0.98</v>
+      </c>
+      <c r="S7">
+        <v>-1.2956294830976989E-2</v>
+      </c>
+      <c r="T7">
+        <v>-2.5679021303599558E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>0.46601743976041099</v>
+      </c>
+      <c r="D8">
+        <v>0.43773578507292599</v>
+      </c>
+      <c r="E8">
+        <v>0.43100040101041798</v>
+      </c>
+      <c r="F8">
+        <v>0.98</v>
+      </c>
+      <c r="G8">
+        <v>0.98</v>
+      </c>
+      <c r="H8">
+        <v>0.98</v>
+      </c>
+      <c r="I8">
+        <v>-3.5017038749993012E-2</v>
+      </c>
+      <c r="J8">
+        <v>-6.7353840625080097E-3</v>
+      </c>
+      <c r="K8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8">
+        <v>8</v>
+      </c>
+      <c r="M8">
+        <v>0.34878544613816698</v>
+      </c>
+      <c r="N8">
+        <v>0.32996034458219498</v>
+      </c>
+      <c r="O8">
+        <v>0.33906997633295999</v>
+      </c>
+      <c r="P8">
+        <v>0.87</v>
+      </c>
+      <c r="Q8">
+        <v>0.93</v>
+      </c>
+      <c r="R8">
+        <v>0.91</v>
+      </c>
+      <c r="S8">
+        <v>-9.7154698052069888E-3</v>
+      </c>
+      <c r="T8">
+        <v>9.1096317507650126E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>0.38238833686615298</v>
+      </c>
+      <c r="D9">
+        <v>0.37643205455844803</v>
+      </c>
+      <c r="E9">
+        <v>0.38083219741125601</v>
+      </c>
+      <c r="F9">
+        <v>0.94</v>
+      </c>
+      <c r="G9">
+        <v>0.95</v>
+      </c>
+      <c r="H9">
+        <v>0.96</v>
+      </c>
+      <c r="I9">
+        <v>-1.5561394548969654E-3</v>
+      </c>
+      <c r="J9">
+        <v>4.4001428528079867E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>0.35597821788773698</v>
+      </c>
+      <c r="D10">
+        <v>0.358426844748505</v>
+      </c>
+      <c r="E10">
+        <v>0.35426868297818498</v>
+      </c>
+      <c r="F10">
+        <v>0.89</v>
+      </c>
+      <c r="G10">
+        <v>0.92</v>
+      </c>
+      <c r="H10">
+        <v>0.96</v>
+      </c>
+      <c r="I10">
+        <v>-1.7095349095520018E-3</v>
+      </c>
+      <c r="J10">
+        <v>-4.1581617703200235E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570351F4-F72D-3549-91BE-BE1BA39081DA}">
+  <dimension ref="A1:T19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:T11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="1" customFormat="1">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.47889802916834801</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.68185850819905403</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.464976153345873</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
         <f>E2-C2</f>
         <v>-1.3921875822475005E-2</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <f>E2-D2</f>
         <v>-0.21688235485318103</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L2">
-        <v>1</v>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.46199256540941303</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0.43366777799214801</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0.44811568913307098</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="S2" s="1">
+        <f>O2-M2</f>
+        <v>-1.3876876276342043E-2</v>
+      </c>
+      <c r="T2" s="1">
+        <f>O2-N2</f>
+        <v>1.4447911140922975E-2</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -607,11 +1219,11 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I10" si="0">E3-C3</f>
+        <f t="shared" ref="I3:I11" si="0">E3-C3</f>
         <v>-4.2677475725760972E-2</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J10" si="1">E3-D3</f>
+        <f t="shared" ref="J3:J11" si="1">E3-D3</f>
         <v>9.3048363975180015E-3</v>
       </c>
       <c r="K3" t="s">
@@ -619,6 +1231,32 @@
       </c>
       <c r="L3">
         <v>2</v>
+      </c>
+      <c r="M3">
+        <v>0.56624871091601903</v>
+      </c>
+      <c r="N3">
+        <v>0.56076166660782301</v>
+      </c>
+      <c r="O3">
+        <v>0.55884107654576798</v>
+      </c>
+      <c r="P3">
+        <v>0.99</v>
+      </c>
+      <c r="Q3">
+        <v>0.99</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S9" si="2">O3-M3</f>
+        <v>-7.4076343702510483E-3</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T9" si="3">O3-N3</f>
+        <v>-1.9205900620550276E-3</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -660,6 +1298,32 @@
       <c r="L4">
         <v>3</v>
       </c>
+      <c r="M4">
+        <v>0.38035551942913998</v>
+      </c>
+      <c r="N4">
+        <v>0.375436632708185</v>
+      </c>
+      <c r="O4">
+        <v>0.37663804515963401</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="2"/>
+        <v>-3.7174742695059715E-3</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="3"/>
+        <v>1.2014124514490021E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
@@ -700,6 +1364,32 @@
       <c r="L5">
         <v>4</v>
       </c>
+      <c r="M5">
+        <v>0.46347544467607799</v>
+      </c>
+      <c r="N5">
+        <v>0.42595182342608801</v>
+      </c>
+      <c r="O5">
+        <v>0.45148728164304902</v>
+      </c>
+      <c r="P5">
+        <v>0.99</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="2"/>
+        <v>-1.1988163033028965E-2</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="3"/>
+        <v>2.5535458216961016E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
@@ -740,6 +1430,32 @@
       <c r="L6">
         <v>5</v>
       </c>
+      <c r="M6">
+        <v>0.47925778126947799</v>
+      </c>
+      <c r="N6">
+        <v>0.44576891401975099</v>
+      </c>
+      <c r="O6">
+        <v>0.45780706597903098</v>
+      </c>
+      <c r="P6">
+        <v>0.99</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="2"/>
+        <v>-2.1450715290447009E-2</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="3"/>
+        <v>1.2038151959279986E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
@@ -780,6 +1496,32 @@
       <c r="L7">
         <v>6</v>
       </c>
+      <c r="M7">
+        <v>0.37286859355993901</v>
+      </c>
+      <c r="N7">
+        <v>0.36248020085932198</v>
+      </c>
+      <c r="O7">
+        <v>0.35991229872896202</v>
+      </c>
+      <c r="P7">
+        <v>0.91</v>
+      </c>
+      <c r="Q7">
+        <v>0.96</v>
+      </c>
+      <c r="R7">
+        <v>0.98</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="2"/>
+        <v>-1.2956294830976989E-2</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="3"/>
+        <v>-2.5679021303599558E-3</v>
+      </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
@@ -820,6 +1562,32 @@
       <c r="L8">
         <v>7</v>
       </c>
+      <c r="M8">
+        <v>0.37286859355993901</v>
+      </c>
+      <c r="N8">
+        <v>0.36248020085932198</v>
+      </c>
+      <c r="O8">
+        <v>0.35991229872896202</v>
+      </c>
+      <c r="P8">
+        <v>0.91</v>
+      </c>
+      <c r="Q8">
+        <v>0.96</v>
+      </c>
+      <c r="R8">
+        <v>0.98</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="2"/>
+        <v>-1.2956294830976989E-2</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="3"/>
+        <v>-2.5679021303599558E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
@@ -854,8 +1622,37 @@
         <f t="shared" si="1"/>
         <v>-6.7353840625080097E-3</v>
       </c>
+      <c r="K9" t="s">
+        <v>29</v>
+      </c>
       <c r="L9">
         <v>8</v>
+      </c>
+      <c r="M9">
+        <v>0.34878544613816698</v>
+      </c>
+      <c r="N9">
+        <v>0.32996034458219498</v>
+      </c>
+      <c r="O9">
+        <v>0.33906997633295999</v>
+      </c>
+      <c r="P9">
+        <v>0.87</v>
+      </c>
+      <c r="Q9">
+        <v>0.93</v>
+      </c>
+      <c r="R9">
+        <v>0.91</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="2"/>
+        <v>-9.7154698052069888E-3</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="3"/>
+        <v>9.1096317507650126E-3</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -893,8 +1690,247 @@
       </c>
     </row>
     <row r="11" spans="1:20">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
       <c r="B11">
         <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.35597821788773698</v>
+      </c>
+      <c r="D11">
+        <v>0.358426844748505</v>
+      </c>
+      <c r="E11">
+        <v>0.35426868297818498</v>
+      </c>
+      <c r="F11">
+        <v>0.89</v>
+      </c>
+      <c r="G11">
+        <v>0.92</v>
+      </c>
+      <c r="H11">
+        <v>0.96</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>-1.7095349095520018E-3</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>-4.1581617703200235E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="C13">
+        <f>AVERAGE(C2:C11)</f>
+        <v>0.45158227370502291</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:T13" si="4">AVERAGE(D2:D11)</f>
+        <v>0.44617464826586373</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="4"/>
+        <v>0.43411910152368122</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>0.96300000000000008</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="4"/>
+        <v>0.9850000000000001</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>-1.7463172181341701E-2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>-1.2055546742182611E-2</v>
+      </c>
+      <c r="K13" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>0.43073158186977156</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>0.41206344513185428</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="4"/>
+        <v>0.41897296653142962</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="4"/>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="4"/>
+        <v>0.97875000000000001</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="4"/>
+        <v>0.98125000000000018</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="4"/>
+        <v>-1.1758615338342E-2</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="4"/>
+        <v>6.9095213995753815E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="C14">
+        <f>AVERAGE(C3:C11)</f>
+        <v>0.44854718976465346</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:T14" si="5">AVERAGE(D3:D11)</f>
+        <v>0.41998755271773158</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="5"/>
+        <v>0.43069054021010433</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="5"/>
+        <v>0.96111111111111114</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>0.98111111111111127</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="5"/>
+        <v>0.98333333333333328</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="5"/>
+        <v>-1.7856649554549114E-2</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="5"/>
+        <v>1.070298749237277E-2</v>
+      </c>
+      <c r="K14" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="5"/>
+        <v>0.42626572707839433</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="5"/>
+        <v>0.40897711186609792</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="5"/>
+        <v>0.41480972044548087</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="5"/>
+        <v>0.9514285714285714</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="5"/>
+        <v>0.97714285714285709</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="5"/>
+        <v>0.98142857142857154</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="5"/>
+        <v>-1.1456006632913423E-2</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="5"/>
+        <v>5.8326085793828685E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="D16">
+        <f>STDEV(D2:D11)</f>
+        <v>9.7752874815885599E-2</v>
+      </c>
+      <c r="E16">
+        <f>STDEV(E2:E11)</f>
+        <v>6.0572474255340465E-2</v>
+      </c>
+      <c r="I16">
+        <f>STDEV(I2:I11)</f>
+        <v>1.6255353176589226E-2</v>
+      </c>
+      <c r="J16">
+        <f>STDEV(J2:J11)</f>
+        <v>7.3303065051272237E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15">
+      <c r="D17">
+        <f>D13+D16*3</f>
+        <v>0.73943327271352055</v>
+      </c>
+      <c r="E17">
+        <f>E13+E16*3</f>
+        <v>0.61583652428970259</v>
+      </c>
+      <c r="I17">
+        <f>I13+I16*3</f>
+        <v>3.130288734842597E-2</v>
+      </c>
+      <c r="J17">
+        <f>J13+J16*3</f>
+        <v>0.20785364841163409</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15">
+      <c r="C19">
+        <f>_xlfn.T.TEST(C3:C11,D3:D11,2,1)</f>
+        <v>1.1496646824547112E-2</v>
+      </c>
+      <c r="D19">
+        <f>_xlfn.T.TEST(D3:D11,E3:E11,2,1)</f>
+        <v>6.1396297841985407E-2</v>
+      </c>
+      <c r="E19">
+        <f>_xlfn.T.TEST(C3:C11,E3:E11,2,1)</f>
+        <v>1.4310775798152993E-2</v>
+      </c>
+      <c r="M19">
+        <f>_xlfn.T.TEST(M3:M11,N3:N11,2,1)</f>
+        <v>1.3826467907335422E-2</v>
+      </c>
+      <c r="N19">
+        <f>_xlfn.T.TEST(N3:N11,O3:O11,2,1)</f>
+        <v>0.19165059207031887</v>
+      </c>
+      <c r="O19">
+        <f>_xlfn.T.TEST(M3:M11,O3:O11,2,1)</f>
+        <v>1.5527454445802961E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>